<commit_message>
TP#15470: Update spreadsheet to get EMEA tests passing
</commit_message>
<xml_diff>
--- a/Code/ShipWorks.Tests.Integration/DataSources/FedExAll/EMEA.xlsx
+++ b/Code/ShipWorks.Tests.Integration/DataSources/FedExAll/EMEA.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1645" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1679" uniqueCount="306">
   <si>
     <t>KG</t>
   </si>
@@ -935,13 +935,25 @@
   </si>
   <si>
     <t>RequestedShipment.RequestedPackageLineItems.SpecialServicesRequested(Repetitions2)</t>
+  </si>
+  <si>
+    <t>HAZARDOUS_MATERIALS</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>123asd789</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1013,8 +1025,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1048,6 +1068,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="62"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1293,7 +1319,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -1427,6 +1453,7 @@
     <xf numFmtId="0" fontId="10" fillId="5" borderId="11" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -1435,6 +1462,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="6" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -1723,10 +1753,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:FE26"/>
+  <dimension ref="A1:FE39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CO1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="CT2" sqref="CT2"/>
+    <sheetView tabSelected="1" topLeftCell="BB1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BI26" sqref="BI26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2751,7 +2781,7 @@
       <c r="A3" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="B3" s="47" t="s">
+      <c r="B3" s="48" t="s">
         <v>152</v>
       </c>
       <c r="C3" s="34" t="s">
@@ -3050,7 +3080,7 @@
       <c r="A4" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="B4" s="48"/>
+      <c r="B4" s="49"/>
       <c r="C4" s="18" t="s">
         <v>145</v>
       </c>
@@ -3381,7 +3411,7 @@
       <c r="A5" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="B5" s="48"/>
+      <c r="B5" s="49"/>
       <c r="C5" s="18" t="s">
         <v>143</v>
       </c>
@@ -3690,7 +3720,7 @@
       <c r="A6" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="B6" s="48"/>
+      <c r="B6" s="49"/>
       <c r="C6" s="18" t="s">
         <v>141</v>
       </c>
@@ -4003,7 +4033,7 @@
       <c r="A7" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="B7" s="48"/>
+      <c r="B7" s="49"/>
       <c r="C7" s="18" t="s">
         <v>139</v>
       </c>
@@ -4326,7 +4356,7 @@
       <c r="A8" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="B8" s="48"/>
+      <c r="B8" s="49"/>
       <c r="C8" s="18" t="s">
         <v>137</v>
       </c>
@@ -4671,7 +4701,7 @@
       <c r="A9" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="B9" s="48"/>
+      <c r="B9" s="49"/>
       <c r="C9" s="18" t="s">
         <v>134</v>
       </c>
@@ -4996,7 +5026,7 @@
       <c r="A10" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="B10" s="48"/>
+      <c r="B10" s="49"/>
       <c r="C10" s="18" t="s">
         <v>131</v>
       </c>
@@ -5305,7 +5335,7 @@
       <c r="A11" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="B11" s="48"/>
+      <c r="B11" s="49"/>
       <c r="C11" s="18" t="s">
         <v>129</v>
       </c>
@@ -5618,7 +5648,7 @@
       <c r="A12" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="B12" s="48"/>
+      <c r="B12" s="49"/>
       <c r="C12" s="18" t="s">
         <v>126</v>
       </c>
@@ -5935,7 +5965,7 @@
       <c r="A13" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="B13" s="48"/>
+      <c r="B13" s="49"/>
       <c r="C13" s="18" t="s">
         <v>124</v>
       </c>
@@ -6272,7 +6302,7 @@
       <c r="A14" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="B14" s="48"/>
+      <c r="B14" s="49"/>
       <c r="C14" s="18" t="s">
         <v>121</v>
       </c>
@@ -6383,9 +6413,15 @@
       <c r="BD14" s="16"/>
       <c r="BE14" s="13"/>
       <c r="BF14" s="13"/>
-      <c r="BG14" s="15"/>
-      <c r="BH14" s="15"/>
-      <c r="BI14" s="15"/>
+      <c r="BG14" s="15" t="s">
+        <v>303</v>
+      </c>
+      <c r="BH14" s="15" t="s">
+        <v>304</v>
+      </c>
+      <c r="BI14" s="15" t="s">
+        <v>305</v>
+      </c>
       <c r="BJ14" s="13"/>
       <c r="BK14" s="13"/>
       <c r="BL14" s="13"/>
@@ -6575,7 +6611,7 @@
       <c r="A15" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="B15" s="48"/>
+      <c r="B15" s="49"/>
       <c r="C15" s="18" t="s">
         <v>119</v>
       </c>
@@ -6690,9 +6726,15 @@
       <c r="BD15" s="16"/>
       <c r="BE15" s="13"/>
       <c r="BF15" s="13"/>
-      <c r="BG15" s="15"/>
-      <c r="BH15" s="15"/>
-      <c r="BI15" s="15"/>
+      <c r="BG15" s="15" t="s">
+        <v>303</v>
+      </c>
+      <c r="BH15" s="15" t="s">
+        <v>304</v>
+      </c>
+      <c r="BI15" s="15" t="s">
+        <v>305</v>
+      </c>
       <c r="BJ15" s="13"/>
       <c r="BK15" s="13"/>
       <c r="BL15" s="13"/>
@@ -6884,7 +6926,7 @@
       <c r="A16" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="B16" s="48"/>
+      <c r="B16" s="49"/>
       <c r="C16" s="18" t="s">
         <v>117</v>
       </c>
@@ -7001,9 +7043,15 @@
       <c r="BD16" s="16"/>
       <c r="BE16" s="13"/>
       <c r="BF16" s="13"/>
-      <c r="BG16" s="15"/>
-      <c r="BH16" s="15"/>
-      <c r="BI16" s="15"/>
+      <c r="BG16" s="15" t="s">
+        <v>303</v>
+      </c>
+      <c r="BH16" s="15" t="s">
+        <v>304</v>
+      </c>
+      <c r="BI16" s="15" t="s">
+        <v>305</v>
+      </c>
       <c r="BJ16" s="13"/>
       <c r="BK16" s="13"/>
       <c r="BL16" s="13"/>
@@ -7197,7 +7245,7 @@
       <c r="A17" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="B17" s="48"/>
+      <c r="B17" s="49"/>
       <c r="C17" s="18" t="s">
         <v>115</v>
       </c>
@@ -7322,9 +7370,15 @@
       <c r="BD17" s="16"/>
       <c r="BE17" s="13"/>
       <c r="BF17" s="13"/>
-      <c r="BG17" s="15"/>
-      <c r="BH17" s="15"/>
-      <c r="BI17" s="15"/>
+      <c r="BG17" s="15" t="s">
+        <v>303</v>
+      </c>
+      <c r="BH17" s="15" t="s">
+        <v>304</v>
+      </c>
+      <c r="BI17" s="15" t="s">
+        <v>305</v>
+      </c>
       <c r="BJ17" s="13"/>
       <c r="BK17" s="13"/>
       <c r="BL17" s="13"/>
@@ -7514,7 +7568,7 @@
       <c r="A18" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="B18" s="48"/>
+      <c r="B18" s="49"/>
       <c r="C18" s="18" t="s">
         <v>113</v>
       </c>
@@ -7627,9 +7681,15 @@
       <c r="BD18" s="16"/>
       <c r="BE18" s="13"/>
       <c r="BF18" s="13"/>
-      <c r="BG18" s="15"/>
-      <c r="BH18" s="15"/>
-      <c r="BI18" s="15"/>
+      <c r="BG18" s="15" t="s">
+        <v>303</v>
+      </c>
+      <c r="BH18" s="15" t="s">
+        <v>304</v>
+      </c>
+      <c r="BI18" s="15" t="s">
+        <v>305</v>
+      </c>
       <c r="BJ18" s="20" t="s">
         <v>109</v>
       </c>
@@ -7676,7 +7736,7 @@
         <v>46</v>
       </c>
       <c r="BY18" s="13" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="BZ18" s="13"/>
       <c r="CA18" s="13"/>
@@ -7851,7 +7911,7 @@
       <c r="A19" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="B19" s="48"/>
+      <c r="B19" s="49"/>
       <c r="C19" s="18" t="s">
         <v>103</v>
       </c>
@@ -7962,9 +8022,15 @@
       <c r="BD19" s="16"/>
       <c r="BE19" s="13"/>
       <c r="BF19" s="13"/>
-      <c r="BG19" s="15"/>
-      <c r="BH19" s="15"/>
-      <c r="BI19" s="15"/>
+      <c r="BG19" s="15" t="s">
+        <v>303</v>
+      </c>
+      <c r="BH19" s="15" t="s">
+        <v>304</v>
+      </c>
+      <c r="BI19" s="15" t="s">
+        <v>305</v>
+      </c>
       <c r="BJ19" s="13"/>
       <c r="BK19" s="13"/>
       <c r="BL19" s="13"/>
@@ -8160,7 +8226,7 @@
       <c r="A20" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="B20" s="48"/>
+      <c r="B20" s="49"/>
       <c r="C20" s="18" t="s">
         <v>99</v>
       </c>
@@ -8275,9 +8341,15 @@
       <c r="BD20" s="16"/>
       <c r="BE20" s="13"/>
       <c r="BF20" s="13"/>
-      <c r="BG20" s="15"/>
-      <c r="BH20" s="15"/>
-      <c r="BI20" s="15"/>
+      <c r="BG20" s="15" t="s">
+        <v>303</v>
+      </c>
+      <c r="BH20" s="15" t="s">
+        <v>304</v>
+      </c>
+      <c r="BI20" s="15" t="s">
+        <v>305</v>
+      </c>
       <c r="BJ20" s="13"/>
       <c r="BK20" s="13"/>
       <c r="BL20" s="13"/>
@@ -8469,7 +8541,7 @@
       <c r="A21" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="B21" s="48"/>
+      <c r="B21" s="49"/>
       <c r="C21" s="18" t="s">
         <v>95</v>
       </c>
@@ -8586,9 +8658,15 @@
       <c r="BD21" s="16"/>
       <c r="BE21" s="13"/>
       <c r="BF21" s="13"/>
-      <c r="BG21" s="15"/>
-      <c r="BH21" s="15"/>
-      <c r="BI21" s="15"/>
+      <c r="BG21" s="15" t="s">
+        <v>303</v>
+      </c>
+      <c r="BH21" s="15" t="s">
+        <v>304</v>
+      </c>
+      <c r="BI21" s="15" t="s">
+        <v>305</v>
+      </c>
       <c r="BJ21" s="13"/>
       <c r="BK21" s="13"/>
       <c r="BL21" s="13"/>
@@ -8782,7 +8860,7 @@
       <c r="A22" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="B22" s="48"/>
+      <c r="B22" s="49"/>
       <c r="C22" s="18" t="s">
         <v>82</v>
       </c>
@@ -8907,9 +8985,15 @@
       <c r="BD22" s="16"/>
       <c r="BE22" s="13"/>
       <c r="BF22" s="13"/>
-      <c r="BG22" s="15"/>
-      <c r="BH22" s="15"/>
-      <c r="BI22" s="15"/>
+      <c r="BG22" s="15" t="s">
+        <v>303</v>
+      </c>
+      <c r="BH22" s="15" t="s">
+        <v>304</v>
+      </c>
+      <c r="BI22" s="15" t="s">
+        <v>305</v>
+      </c>
       <c r="BJ22" s="13"/>
       <c r="BK22" s="13"/>
       <c r="BL22" s="13"/>
@@ -9099,7 +9183,7 @@
       <c r="A23" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="B23" s="48"/>
+      <c r="B23" s="49"/>
       <c r="C23" s="18" t="s">
         <v>73</v>
       </c>
@@ -9232,9 +9316,15 @@
       <c r="BF23" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="BG23" s="15"/>
-      <c r="BH23" s="15"/>
-      <c r="BI23" s="15"/>
+      <c r="BG23" s="15" t="s">
+        <v>303</v>
+      </c>
+      <c r="BH23" s="15" t="s">
+        <v>304</v>
+      </c>
+      <c r="BI23" s="15" t="s">
+        <v>305</v>
+      </c>
       <c r="BJ23" s="20"/>
       <c r="BK23" s="14"/>
       <c r="BL23" s="20"/>
@@ -9424,7 +9514,7 @@
       <c r="A24" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="B24" s="48"/>
+      <c r="B24" s="49"/>
       <c r="C24" s="18" t="s">
         <v>63</v>
       </c>
@@ -9767,7 +9857,7 @@
       <c r="A25" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="B25" s="48"/>
+      <c r="B25" s="49"/>
       <c r="C25" s="18" t="s">
         <v>53</v>
       </c>
@@ -10055,7 +10145,9 @@
       <c r="EM25" s="12">
         <v>0</v>
       </c>
-      <c r="EN25" s="12"/>
+      <c r="EN25" s="51" t="s">
+        <v>302</v>
+      </c>
       <c r="EO25" s="12" t="s">
         <v>7</v>
       </c>
@@ -10112,7 +10204,7 @@
       <c r="A26" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="B26" s="49"/>
+      <c r="B26" s="50"/>
       <c r="C26" s="9" t="s">
         <v>43</v>
       </c>
@@ -10223,9 +10315,15 @@
       <c r="BD26" s="8"/>
       <c r="BE26" s="6"/>
       <c r="BF26" s="6"/>
-      <c r="BG26" s="7"/>
-      <c r="BH26" s="7"/>
-      <c r="BI26" s="7"/>
+      <c r="BG26" s="7" t="s">
+        <v>303</v>
+      </c>
+      <c r="BH26" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="BI26" s="15" t="s">
+        <v>305</v>
+      </c>
       <c r="BJ26" s="6"/>
       <c r="BK26" s="6"/>
       <c r="BL26" s="6"/>
@@ -10453,6 +10551,9 @@
         <v>9015551234</v>
       </c>
     </row>
+    <row r="39" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F39" s="47"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B3:B26"/>

</xml_diff>

<commit_message>
TP#15470: Update EMEA spreadsheet
</commit_message>
<xml_diff>
--- a/Code/ShipWorks.Tests.Integration/DataSources/FedExAll/EMEA.xlsx
+++ b/Code/ShipWorks.Tests.Integration/DataSources/FedExAll/EMEA.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1679" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1677" uniqueCount="306">
   <si>
     <t>KG</t>
   </si>
@@ -1454,6 +1454,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="6" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -1462,9 +1465,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="6" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -1755,63 +1755,63 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:FE39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BB1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BI26" sqref="BI26"/>
+    <sheetView tabSelected="1" topLeftCell="CE1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="CI14" sqref="CI14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.125" style="1"/>
-    <col min="2" max="2" width="9.125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="52.625" style="1" customWidth="1"/>
-    <col min="4" max="12" width="30.75" style="1" customWidth="1"/>
-    <col min="13" max="13" width="22.75" style="1" customWidth="1"/>
-    <col min="14" max="14" width="30.625" style="1" customWidth="1"/>
-    <col min="15" max="16" width="20.75" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="9.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="52.5703125" style="1" customWidth="1"/>
+    <col min="4" max="12" width="30.7109375" style="1" customWidth="1"/>
+    <col min="13" max="13" width="22.7109375" style="1" customWidth="1"/>
+    <col min="14" max="14" width="30.5703125" style="1" customWidth="1"/>
+    <col min="15" max="16" width="20.7109375" style="1" customWidth="1"/>
     <col min="17" max="17" width="15" style="1" customWidth="1"/>
-    <col min="18" max="18" width="30.75" style="1" customWidth="1"/>
-    <col min="19" max="19" width="17.125" style="1" customWidth="1"/>
-    <col min="20" max="20" width="26.375" style="1" customWidth="1"/>
-    <col min="21" max="21" width="23.625" style="1" customWidth="1"/>
-    <col min="22" max="22" width="20.75" style="1" customWidth="1"/>
-    <col min="23" max="23" width="19.125" style="1" customWidth="1"/>
-    <col min="24" max="24" width="20.25" style="1" customWidth="1"/>
-    <col min="25" max="25" width="25.125" style="1" customWidth="1"/>
-    <col min="26" max="26" width="20.125" style="1" customWidth="1"/>
-    <col min="27" max="27" width="22.125" style="1" customWidth="1"/>
-    <col min="28" max="28" width="30.75" style="1" customWidth="1"/>
-    <col min="29" max="29" width="25.25" style="1" customWidth="1"/>
-    <col min="30" max="30" width="21.25" style="1" customWidth="1"/>
-    <col min="31" max="31" width="19.25" style="1" customWidth="1"/>
-    <col min="32" max="32" width="23.375" style="1" customWidth="1"/>
-    <col min="33" max="33" width="15.25" style="1" customWidth="1"/>
-    <col min="34" max="34" width="16.125" style="1" customWidth="1"/>
-    <col min="35" max="35" width="27.75" style="1" customWidth="1"/>
-    <col min="36" max="40" width="20.75" style="1" customWidth="1"/>
-    <col min="41" max="41" width="36.25" style="1" customWidth="1"/>
-    <col min="42" max="81" width="20.75" style="1" customWidth="1"/>
-    <col min="82" max="82" width="37.875" style="1" customWidth="1"/>
-    <col min="83" max="122" width="20.75" style="1" customWidth="1"/>
-    <col min="123" max="123" width="13.25" style="1" customWidth="1"/>
-    <col min="124" max="124" width="16.125" style="1" customWidth="1"/>
-    <col min="125" max="139" width="20.75" style="1" customWidth="1"/>
-    <col min="140" max="147" width="30.75" style="1" customWidth="1"/>
-    <col min="148" max="148" width="14.625" style="1" customWidth="1"/>
-    <col min="149" max="149" width="11.875" style="1" customWidth="1"/>
-    <col min="150" max="150" width="13.5" style="1" customWidth="1"/>
+    <col min="18" max="18" width="30.7109375" style="1" customWidth="1"/>
+    <col min="19" max="19" width="17.140625" style="1" customWidth="1"/>
+    <col min="20" max="20" width="26.42578125" style="1" customWidth="1"/>
+    <col min="21" max="21" width="23.5703125" style="1" customWidth="1"/>
+    <col min="22" max="22" width="20.7109375" style="1" customWidth="1"/>
+    <col min="23" max="23" width="19.140625" style="1" customWidth="1"/>
+    <col min="24" max="24" width="20.28515625" style="1" customWidth="1"/>
+    <col min="25" max="25" width="25.140625" style="1" customWidth="1"/>
+    <col min="26" max="26" width="20.140625" style="1" customWidth="1"/>
+    <col min="27" max="27" width="22.140625" style="1" customWidth="1"/>
+    <col min="28" max="28" width="30.7109375" style="1" customWidth="1"/>
+    <col min="29" max="29" width="25.28515625" style="1" customWidth="1"/>
+    <col min="30" max="30" width="21.28515625" style="1" customWidth="1"/>
+    <col min="31" max="31" width="19.28515625" style="1" customWidth="1"/>
+    <col min="32" max="32" width="23.42578125" style="1" customWidth="1"/>
+    <col min="33" max="33" width="15.28515625" style="1" customWidth="1"/>
+    <col min="34" max="34" width="16.140625" style="1" customWidth="1"/>
+    <col min="35" max="35" width="27.7109375" style="1" customWidth="1"/>
+    <col min="36" max="40" width="20.7109375" style="1" customWidth="1"/>
+    <col min="41" max="41" width="36.28515625" style="1" customWidth="1"/>
+    <col min="42" max="81" width="20.7109375" style="1" customWidth="1"/>
+    <col min="82" max="82" width="37.85546875" style="1" customWidth="1"/>
+    <col min="83" max="122" width="20.7109375" style="1" customWidth="1"/>
+    <col min="123" max="123" width="13.28515625" style="1" customWidth="1"/>
+    <col min="124" max="124" width="16.140625" style="1" customWidth="1"/>
+    <col min="125" max="139" width="20.7109375" style="1" customWidth="1"/>
+    <col min="140" max="147" width="30.7109375" style="1" customWidth="1"/>
+    <col min="148" max="148" width="14.5703125" style="1" customWidth="1"/>
+    <col min="149" max="149" width="11.85546875" style="1" customWidth="1"/>
+    <col min="150" max="150" width="13.42578125" style="1" customWidth="1"/>
     <col min="151" max="151" width="13" style="1" customWidth="1"/>
-    <col min="152" max="152" width="14.25" style="1" customWidth="1"/>
-    <col min="153" max="153" width="13.125" style="1" customWidth="1"/>
-    <col min="154" max="154" width="14.5" style="1" customWidth="1"/>
-    <col min="155" max="155" width="13.375" style="1" customWidth="1"/>
+    <col min="152" max="152" width="14.28515625" style="1" customWidth="1"/>
+    <col min="153" max="153" width="13.140625" style="1" customWidth="1"/>
+    <col min="154" max="154" width="14.42578125" style="1" customWidth="1"/>
+    <col min="155" max="155" width="13.42578125" style="1" customWidth="1"/>
     <col min="156" max="156" width="14" style="1" customWidth="1"/>
-    <col min="157" max="157" width="15.75" style="1" customWidth="1"/>
-    <col min="158" max="158" width="17.125" style="1" customWidth="1"/>
+    <col min="157" max="157" width="15.7109375" style="1" customWidth="1"/>
+    <col min="158" max="158" width="17.140625" style="1" customWidth="1"/>
     <col min="159" max="159" width="13" style="1" customWidth="1"/>
-    <col min="160" max="160" width="16.625" style="1" customWidth="1"/>
-    <col min="161" max="162" width="24.375" style="1" customWidth="1"/>
-    <col min="163" max="163" width="30.75" style="1" customWidth="1"/>
-    <col min="164" max="16384" width="9.125" style="1"/>
+    <col min="160" max="160" width="16.5703125" style="1" customWidth="1"/>
+    <col min="161" max="162" width="24.42578125" style="1" customWidth="1"/>
+    <col min="163" max="163" width="30.7109375" style="1" customWidth="1"/>
+    <col min="164" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:161" s="35" customFormat="1" ht="172.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2781,7 +2781,7 @@
       <c r="A3" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="B3" s="48" t="s">
+      <c r="B3" s="49" t="s">
         <v>152</v>
       </c>
       <c r="C3" s="34" t="s">
@@ -3080,7 +3080,7 @@
       <c r="A4" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="B4" s="49"/>
+      <c r="B4" s="50"/>
       <c r="C4" s="18" t="s">
         <v>145</v>
       </c>
@@ -3411,7 +3411,7 @@
       <c r="A5" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="B5" s="49"/>
+      <c r="B5" s="50"/>
       <c r="C5" s="18" t="s">
         <v>143</v>
       </c>
@@ -3720,7 +3720,7 @@
       <c r="A6" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="B6" s="49"/>
+      <c r="B6" s="50"/>
       <c r="C6" s="18" t="s">
         <v>141</v>
       </c>
@@ -4033,7 +4033,7 @@
       <c r="A7" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="B7" s="49"/>
+      <c r="B7" s="50"/>
       <c r="C7" s="18" t="s">
         <v>139</v>
       </c>
@@ -4177,9 +4177,7 @@
       <c r="BW7" s="14"/>
       <c r="BX7" s="14"/>
       <c r="BY7" s="14"/>
-      <c r="BZ7" s="13" t="s">
-        <v>96</v>
-      </c>
+      <c r="BZ7" s="13"/>
       <c r="CA7" s="14"/>
       <c r="CB7" s="14"/>
       <c r="CC7" s="14"/>
@@ -4192,12 +4190,8 @@
       <c r="CJ7" s="14"/>
       <c r="CK7" s="14"/>
       <c r="CL7" s="14"/>
-      <c r="CM7" s="14" t="s">
-        <v>135</v>
-      </c>
-      <c r="CN7" s="14">
-        <v>12345678</v>
-      </c>
+      <c r="CM7" s="14"/>
+      <c r="CN7" s="14"/>
       <c r="CO7" s="14" t="s">
         <v>26</v>
       </c>
@@ -4356,7 +4350,7 @@
       <c r="A8" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="B8" s="49"/>
+      <c r="B8" s="50"/>
       <c r="C8" s="18" t="s">
         <v>137</v>
       </c>
@@ -4701,7 +4695,7 @@
       <c r="A9" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="B9" s="49"/>
+      <c r="B9" s="50"/>
       <c r="C9" s="18" t="s">
         <v>134</v>
       </c>
@@ -5026,7 +5020,7 @@
       <c r="A10" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="B10" s="49"/>
+      <c r="B10" s="50"/>
       <c r="C10" s="18" t="s">
         <v>131</v>
       </c>
@@ -5335,7 +5329,7 @@
       <c r="A11" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="B11" s="49"/>
+      <c r="B11" s="50"/>
       <c r="C11" s="18" t="s">
         <v>129</v>
       </c>
@@ -5648,7 +5642,7 @@
       <c r="A12" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="B12" s="49"/>
+      <c r="B12" s="50"/>
       <c r="C12" s="18" t="s">
         <v>126</v>
       </c>
@@ -5965,7 +5959,7 @@
       <c r="A13" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="B13" s="49"/>
+      <c r="B13" s="50"/>
       <c r="C13" s="18" t="s">
         <v>124</v>
       </c>
@@ -6302,7 +6296,7 @@
       <c r="A14" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="B14" s="49"/>
+      <c r="B14" s="50"/>
       <c r="C14" s="18" t="s">
         <v>121</v>
       </c>
@@ -6611,7 +6605,7 @@
       <c r="A15" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="B15" s="49"/>
+      <c r="B15" s="50"/>
       <c r="C15" s="18" t="s">
         <v>119</v>
       </c>
@@ -6926,7 +6920,7 @@
       <c r="A16" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="B16" s="49"/>
+      <c r="B16" s="50"/>
       <c r="C16" s="18" t="s">
         <v>117</v>
       </c>
@@ -7245,7 +7239,7 @@
       <c r="A17" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="B17" s="49"/>
+      <c r="B17" s="50"/>
       <c r="C17" s="18" t="s">
         <v>115</v>
       </c>
@@ -7568,7 +7562,7 @@
       <c r="A18" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="B18" s="49"/>
+      <c r="B18" s="50"/>
       <c r="C18" s="18" t="s">
         <v>113</v>
       </c>
@@ -7911,7 +7905,7 @@
       <c r="A19" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="B19" s="49"/>
+      <c r="B19" s="50"/>
       <c r="C19" s="18" t="s">
         <v>103</v>
       </c>
@@ -8226,7 +8220,7 @@
       <c r="A20" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="B20" s="49"/>
+      <c r="B20" s="50"/>
       <c r="C20" s="18" t="s">
         <v>99</v>
       </c>
@@ -8541,7 +8535,7 @@
       <c r="A21" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="B21" s="49"/>
+      <c r="B21" s="50"/>
       <c r="C21" s="18" t="s">
         <v>95</v>
       </c>
@@ -8860,7 +8854,7 @@
       <c r="A22" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="B22" s="49"/>
+      <c r="B22" s="50"/>
       <c r="C22" s="18" t="s">
         <v>82</v>
       </c>
@@ -9183,7 +9177,7 @@
       <c r="A23" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="B23" s="49"/>
+      <c r="B23" s="50"/>
       <c r="C23" s="18" t="s">
         <v>73</v>
       </c>
@@ -9514,7 +9508,7 @@
       <c r="A24" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="B24" s="49"/>
+      <c r="B24" s="50"/>
       <c r="C24" s="18" t="s">
         <v>63</v>
       </c>
@@ -9857,7 +9851,7 @@
       <c r="A25" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="B25" s="49"/>
+      <c r="B25" s="50"/>
       <c r="C25" s="18" t="s">
         <v>53</v>
       </c>
@@ -10145,7 +10139,7 @@
       <c r="EM25" s="12">
         <v>0</v>
       </c>
-      <c r="EN25" s="51" t="s">
+      <c r="EN25" s="48" t="s">
         <v>302</v>
       </c>
       <c r="EO25" s="12" t="s">
@@ -10204,7 +10198,7 @@
       <c r="A26" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="B26" s="50"/>
+      <c r="B26" s="51"/>
       <c r="C26" s="9" t="s">
         <v>43</v>
       </c>

</xml_diff>

<commit_message>
TP#15470: Update fixtures to use correct state code
</commit_message>
<xml_diff>
--- a/Code/ShipWorks.Tests.Integration/DataSources/FedExAll/EMEA.xlsx
+++ b/Code/ShipWorks.Tests.Integration/DataSources/FedExAll/EMEA.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1677" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1680" uniqueCount="305">
   <si>
     <t>KG</t>
   </si>
@@ -935,9 +935,6 @@
   </si>
   <si>
     <t>RequestedShipment.RequestedPackageLineItems.SpecialServicesRequested(Repetitions2)</t>
-  </si>
-  <si>
-    <t>HAZARDOUS_MATERIALS</t>
   </si>
   <si>
     <t>1</t>
@@ -1755,8 +1752,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:FE39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CE1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="CI14" sqref="CI14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4518,7 +4515,9 @@
       <c r="BY8" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="BZ8" s="14"/>
+      <c r="BZ8" s="13" t="s">
+        <v>96</v>
+      </c>
       <c r="CA8" s="14"/>
       <c r="CB8" s="14"/>
       <c r="CC8" s="14"/>
@@ -6408,13 +6407,13 @@
       <c r="BE14" s="13"/>
       <c r="BF14" s="13"/>
       <c r="BG14" s="15" t="s">
+        <v>302</v>
+      </c>
+      <c r="BH14" s="15" t="s">
         <v>303</v>
       </c>
-      <c r="BH14" s="15" t="s">
+      <c r="BI14" s="15" t="s">
         <v>304</v>
-      </c>
-      <c r="BI14" s="15" t="s">
-        <v>305</v>
       </c>
       <c r="BJ14" s="13"/>
       <c r="BK14" s="13"/>
@@ -6721,13 +6720,13 @@
       <c r="BE15" s="13"/>
       <c r="BF15" s="13"/>
       <c r="BG15" s="15" t="s">
+        <v>302</v>
+      </c>
+      <c r="BH15" s="15" t="s">
         <v>303</v>
       </c>
-      <c r="BH15" s="15" t="s">
+      <c r="BI15" s="15" t="s">
         <v>304</v>
-      </c>
-      <c r="BI15" s="15" t="s">
-        <v>305</v>
       </c>
       <c r="BJ15" s="13"/>
       <c r="BK15" s="13"/>
@@ -7038,13 +7037,13 @@
       <c r="BE16" s="13"/>
       <c r="BF16" s="13"/>
       <c r="BG16" s="15" t="s">
+        <v>302</v>
+      </c>
+      <c r="BH16" s="15" t="s">
         <v>303</v>
       </c>
-      <c r="BH16" s="15" t="s">
+      <c r="BI16" s="15" t="s">
         <v>304</v>
-      </c>
-      <c r="BI16" s="15" t="s">
-        <v>305</v>
       </c>
       <c r="BJ16" s="13"/>
       <c r="BK16" s="13"/>
@@ -7365,13 +7364,13 @@
       <c r="BE17" s="13"/>
       <c r="BF17" s="13"/>
       <c r="BG17" s="15" t="s">
+        <v>302</v>
+      </c>
+      <c r="BH17" s="15" t="s">
         <v>303</v>
       </c>
-      <c r="BH17" s="15" t="s">
+      <c r="BI17" s="15" t="s">
         <v>304</v>
-      </c>
-      <c r="BI17" s="15" t="s">
-        <v>305</v>
       </c>
       <c r="BJ17" s="13"/>
       <c r="BK17" s="13"/>
@@ -7676,13 +7675,13 @@
       <c r="BE18" s="13"/>
       <c r="BF18" s="13"/>
       <c r="BG18" s="15" t="s">
+        <v>302</v>
+      </c>
+      <c r="BH18" s="15" t="s">
         <v>303</v>
       </c>
-      <c r="BH18" s="15" t="s">
+      <c r="BI18" s="15" t="s">
         <v>304</v>
-      </c>
-      <c r="BI18" s="15" t="s">
-        <v>305</v>
       </c>
       <c r="BJ18" s="20" t="s">
         <v>109</v>
@@ -8017,13 +8016,13 @@
       <c r="BE19" s="13"/>
       <c r="BF19" s="13"/>
       <c r="BG19" s="15" t="s">
+        <v>302</v>
+      </c>
+      <c r="BH19" s="15" t="s">
         <v>303</v>
       </c>
-      <c r="BH19" s="15" t="s">
+      <c r="BI19" s="15" t="s">
         <v>304</v>
-      </c>
-      <c r="BI19" s="15" t="s">
-        <v>305</v>
       </c>
       <c r="BJ19" s="13"/>
       <c r="BK19" s="13"/>
@@ -8336,13 +8335,13 @@
       <c r="BE20" s="13"/>
       <c r="BF20" s="13"/>
       <c r="BG20" s="15" t="s">
+        <v>302</v>
+      </c>
+      <c r="BH20" s="15" t="s">
         <v>303</v>
       </c>
-      <c r="BH20" s="15" t="s">
+      <c r="BI20" s="15" t="s">
         <v>304</v>
-      </c>
-      <c r="BI20" s="15" t="s">
-        <v>305</v>
       </c>
       <c r="BJ20" s="13"/>
       <c r="BK20" s="13"/>
@@ -8653,13 +8652,13 @@
       <c r="BE21" s="13"/>
       <c r="BF21" s="13"/>
       <c r="BG21" s="15" t="s">
+        <v>302</v>
+      </c>
+      <c r="BH21" s="15" t="s">
         <v>303</v>
       </c>
-      <c r="BH21" s="15" t="s">
+      <c r="BI21" s="15" t="s">
         <v>304</v>
-      </c>
-      <c r="BI21" s="15" t="s">
-        <v>305</v>
       </c>
       <c r="BJ21" s="13"/>
       <c r="BK21" s="13"/>
@@ -8980,13 +8979,13 @@
       <c r="BE22" s="13"/>
       <c r="BF22" s="13"/>
       <c r="BG22" s="15" t="s">
+        <v>302</v>
+      </c>
+      <c r="BH22" s="15" t="s">
         <v>303</v>
       </c>
-      <c r="BH22" s="15" t="s">
+      <c r="BI22" s="15" t="s">
         <v>304</v>
-      </c>
-      <c r="BI22" s="15" t="s">
-        <v>305</v>
       </c>
       <c r="BJ22" s="13"/>
       <c r="BK22" s="13"/>
@@ -9311,13 +9310,13 @@
         <v>65</v>
       </c>
       <c r="BG23" s="15" t="s">
+        <v>302</v>
+      </c>
+      <c r="BH23" s="15" t="s">
         <v>303</v>
       </c>
-      <c r="BH23" s="15" t="s">
+      <c r="BI23" s="15" t="s">
         <v>304</v>
-      </c>
-      <c r="BI23" s="15" t="s">
-        <v>305</v>
       </c>
       <c r="BJ23" s="20"/>
       <c r="BK23" s="14"/>
@@ -9866,7 +9865,7 @@
         <v>41</v>
       </c>
       <c r="H25" s="15" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="I25" s="15" t="s">
         <v>39</v>
@@ -9962,9 +9961,15 @@
       <c r="BD25" s="16"/>
       <c r="BE25" s="13"/>
       <c r="BF25" s="13"/>
-      <c r="BG25" s="15"/>
-      <c r="BH25" s="15"/>
-      <c r="BI25" s="15"/>
+      <c r="BG25" s="15" t="s">
+        <v>302</v>
+      </c>
+      <c r="BH25" s="15" t="s">
+        <v>303</v>
+      </c>
+      <c r="BI25" s="15" t="s">
+        <v>304</v>
+      </c>
       <c r="BJ25" s="13"/>
       <c r="BK25" s="13"/>
       <c r="BL25" s="13"/>
@@ -10139,9 +10144,7 @@
       <c r="EM25" s="12">
         <v>0</v>
       </c>
-      <c r="EN25" s="48" t="s">
-        <v>302</v>
-      </c>
+      <c r="EN25" s="48"/>
       <c r="EO25" s="12" t="s">
         <v>7</v>
       </c>
@@ -10310,13 +10313,13 @@
       <c r="BE26" s="6"/>
       <c r="BF26" s="6"/>
       <c r="BG26" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="BH26" s="7" t="s">
         <v>303</v>
       </c>
-      <c r="BH26" s="7" t="s">
+      <c r="BI26" s="15" t="s">
         <v>304</v>
-      </c>
-      <c r="BI26" s="15" t="s">
-        <v>305</v>
       </c>
       <c r="BJ26" s="6"/>
       <c r="BK26" s="6"/>

</xml_diff>

<commit_message>
TP#20088: EMEA FedEx cert
</commit_message>
<xml_diff>
--- a/Code/ShipWorks.Tests.Integration/DataSources/FedExAll/EMEA.xlsx
+++ b/Code/ShipWorks.Tests.Integration/DataSources/FedExAll/EMEA.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18625"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwinchester\Documents\ShipWorks3x\Code\ShipWorks.Tests.Integration\DataSources\FedExAll\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\ShipWorks\Code\ShipWorks.Tests.Integration\DataSources\FedExAll\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,12 +19,12 @@
     <definedName name="_lu1">#REF!</definedName>
     <definedName name="_lu2">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1782" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1759" uniqueCount="317">
   <si>
     <t>Description</t>
   </si>
@@ -929,9 +929,6 @@
     <t>Intl Priority, Your Packaging, IDG, Dry Ice</t>
   </si>
   <si>
-    <t>Current System Date</t>
-  </si>
-  <si>
     <t>Intl Priority Freight, Your Packaging, HAL</t>
   </si>
   <si>
@@ -969,12 +966,21 @@
   </si>
   <si>
     <t>SaveLabel</t>
+  </si>
+  <si>
+    <t>RequestedShipment.RequestedPackageLineItems.SpecialServicesRequested(Repetitions2)</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>123456</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1971,6 +1977,7 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="18" xfId="360" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="13" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="12" xfId="13" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
@@ -1989,7 +1996,6 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="14" xfId="13" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="13" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="383">
     <cellStyle name="Hyperlink 2" xfId="365"/>
@@ -2477,23 +2483,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2529,23 +2518,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2725,8 +2697,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:FH27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2774,7 +2746,7 @@
   <sheetData>
     <row r="1" spans="1:164" s="7" customFormat="1" ht="69.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="69" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B1" s="68"/>
       <c r="C1" s="5" t="s">
@@ -3192,7 +3164,7 @@
         <v>55</v>
       </c>
       <c r="EK1" s="5" t="s">
-        <v>55</v>
+        <v>314</v>
       </c>
       <c r="EL1" s="5" t="s">
         <v>56</v>
@@ -3264,7 +3236,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:164" s="7" customFormat="1" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:164" s="7" customFormat="1" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="71"/>
       <c r="B2" s="70"/>
       <c r="C2" s="8"/>
@@ -3751,11 +3723,11 @@
       </c>
     </row>
     <row r="3" spans="1:164" s="11" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="78" t="b">
+      <c r="A3" s="72" t="b">
         <v>0</v>
       </c>
-      <c r="B3" s="72" t="s">
-        <v>311</v>
+      <c r="B3" s="73" t="s">
+        <v>310</v>
       </c>
       <c r="C3" s="23" t="s">
         <v>259</v>
@@ -3766,9 +3738,7 @@
       <c r="E3" s="16" t="s">
         <v>169</v>
       </c>
-      <c r="F3" s="16" t="s">
-        <v>301</v>
-      </c>
+      <c r="F3" s="16"/>
       <c r="G3" s="16" t="s">
         <v>162</v>
       </c>
@@ -4075,10 +4045,10 @@
       <c r="FH3" s="27"/>
     </row>
     <row r="4" spans="1:164" s="12" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="78" t="b">
+      <c r="A4" s="72" t="b">
         <v>0</v>
       </c>
-      <c r="B4" s="73"/>
+      <c r="B4" s="74"/>
       <c r="C4" s="23" t="s">
         <v>222</v>
       </c>
@@ -4088,9 +4058,7 @@
       <c r="E4" s="16" t="s">
         <v>174</v>
       </c>
-      <c r="F4" s="16" t="s">
-        <v>301</v>
-      </c>
+      <c r="F4" s="16"/>
       <c r="G4" s="29" t="s">
         <v>162</v>
       </c>
@@ -4407,10 +4375,10 @@
       <c r="FH4" s="34"/>
     </row>
     <row r="5" spans="1:164" s="12" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="78" t="b">
+      <c r="A5" s="72" t="b">
         <v>0</v>
       </c>
-      <c r="B5" s="73"/>
+      <c r="B5" s="74"/>
       <c r="C5" s="23" t="s">
         <v>291</v>
       </c>
@@ -4420,9 +4388,7 @@
       <c r="E5" s="16" t="s">
         <v>175</v>
       </c>
-      <c r="F5" s="16" t="s">
-        <v>301</v>
-      </c>
+      <c r="F5" s="16"/>
       <c r="G5" s="29" t="s">
         <v>162</v>
       </c>
@@ -4609,16 +4575,16 @@
         <v>165</v>
       </c>
       <c r="CJ5" s="29" t="s">
+        <v>303</v>
+      </c>
+      <c r="CK5" s="29" t="s">
         <v>304</v>
-      </c>
-      <c r="CK5" s="29" t="s">
-        <v>305</v>
       </c>
       <c r="CL5" s="29">
         <v>8022</v>
       </c>
       <c r="CM5" s="29" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="CN5" s="29" t="s">
         <v>229</v>
@@ -4785,10 +4751,10 @@
       <c r="FH5" s="34"/>
     </row>
     <row r="6" spans="1:164" s="11" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="78" t="b">
+      <c r="A6" s="72" t="b">
         <v>0</v>
       </c>
-      <c r="B6" s="73"/>
+      <c r="B6" s="74"/>
       <c r="C6" s="23" t="s">
         <v>260</v>
       </c>
@@ -4798,9 +4764,7 @@
       <c r="E6" s="16" t="s">
         <v>176</v>
       </c>
-      <c r="F6" s="16" t="s">
-        <v>301</v>
-      </c>
+      <c r="F6" s="16"/>
       <c r="G6" s="16" t="s">
         <v>162</v>
       </c>
@@ -5119,10 +5083,10 @@
       <c r="FH6" s="27"/>
     </row>
     <row r="7" spans="1:164" s="11" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="78" t="b">
+      <c r="A7" s="72" t="b">
         <v>0</v>
       </c>
-      <c r="B7" s="73"/>
+      <c r="B7" s="74"/>
       <c r="C7" s="23" t="s">
         <v>261</v>
       </c>
@@ -5132,9 +5096,7 @@
       <c r="E7" s="16" t="s">
         <v>180</v>
       </c>
-      <c r="F7" s="16" t="s">
-        <v>301</v>
-      </c>
+      <c r="F7" s="16"/>
       <c r="G7" s="16" t="s">
         <v>162</v>
       </c>
@@ -5437,10 +5399,10 @@
       <c r="FH7" s="27"/>
     </row>
     <row r="8" spans="1:164" s="11" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="78" t="b">
+      <c r="A8" s="72" t="b">
         <v>0</v>
       </c>
-      <c r="B8" s="73"/>
+      <c r="B8" s="74"/>
       <c r="C8" s="23" t="s">
         <v>262</v>
       </c>
@@ -5450,9 +5412,7 @@
       <c r="E8" s="16" t="s">
         <v>199</v>
       </c>
-      <c r="F8" s="16" t="s">
-        <v>301</v>
-      </c>
+      <c r="F8" s="16"/>
       <c r="G8" s="16" t="s">
         <v>162</v>
       </c>
@@ -5759,10 +5719,10 @@
       <c r="FH8" s="27"/>
     </row>
     <row r="9" spans="1:164" s="11" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="78" t="b">
+      <c r="A9" s="72" t="b">
         <v>0</v>
       </c>
-      <c r="B9" s="73"/>
+      <c r="B9" s="74"/>
       <c r="C9" s="23" t="s">
         <v>230</v>
       </c>
@@ -5772,9 +5732,7 @@
       <c r="E9" s="16" t="s">
         <v>200</v>
       </c>
-      <c r="F9" s="16" t="s">
-        <v>301</v>
-      </c>
+      <c r="F9" s="16"/>
       <c r="G9" s="16" t="s">
         <v>162</v>
       </c>
@@ -6085,10 +6043,10 @@
       <c r="FH9" s="27"/>
     </row>
     <row r="10" spans="1:164" s="11" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="78" t="b">
+      <c r="A10" s="72" t="b">
         <v>0</v>
       </c>
-      <c r="B10" s="73"/>
+      <c r="B10" s="74"/>
       <c r="C10" s="23" t="s">
         <v>297</v>
       </c>
@@ -6098,9 +6056,7 @@
       <c r="E10" s="16" t="s">
         <v>201</v>
       </c>
-      <c r="F10" s="16" t="s">
-        <v>301</v>
-      </c>
+      <c r="F10" s="16"/>
       <c r="G10" s="16" t="s">
         <v>162</v>
       </c>
@@ -6397,10 +6353,10 @@
       <c r="FH10" s="27"/>
     </row>
     <row r="11" spans="1:164" s="11" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="78" t="b">
+      <c r="A11" s="72" t="b">
         <v>0</v>
       </c>
-      <c r="B11" s="73"/>
+      <c r="B11" s="74"/>
       <c r="C11" s="23" t="s">
         <v>264</v>
       </c>
@@ -6410,9 +6366,7 @@
       <c r="E11" s="16" t="s">
         <v>202</v>
       </c>
-      <c r="F11" s="16" t="s">
-        <v>301</v>
-      </c>
+      <c r="F11" s="16"/>
       <c r="G11" s="16" t="s">
         <v>162</v>
       </c>
@@ -6715,10 +6669,10 @@
       <c r="FH11" s="27"/>
     </row>
     <row r="12" spans="1:164" s="11" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="78" t="b">
+      <c r="A12" s="72" t="b">
         <v>0</v>
       </c>
-      <c r="B12" s="73"/>
+      <c r="B12" s="74"/>
       <c r="C12" s="23" t="s">
         <v>265</v>
       </c>
@@ -6728,9 +6682,7 @@
       <c r="E12" s="16" t="s">
         <v>203</v>
       </c>
-      <c r="F12" s="16" t="s">
-        <v>301</v>
-      </c>
+      <c r="F12" s="16"/>
       <c r="G12" s="16" t="s">
         <v>162</v>
       </c>
@@ -7037,12 +6989,12 @@
       <c r="FH12" s="27"/>
     </row>
     <row r="13" spans="1:164" s="11" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="78" t="b">
+      <c r="A13" s="72" t="b">
         <v>0</v>
       </c>
-      <c r="B13" s="73"/>
+      <c r="B13" s="74"/>
       <c r="C13" s="23" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D13" s="24" t="s">
         <v>140</v>
@@ -7050,9 +7002,7 @@
       <c r="E13" s="16" t="s">
         <v>207</v>
       </c>
-      <c r="F13" s="16" t="s">
-        <v>301</v>
-      </c>
+      <c r="F13" s="16"/>
       <c r="G13" s="16" t="s">
         <v>162</v>
       </c>
@@ -7363,10 +7313,10 @@
       <c r="FH13" s="27"/>
     </row>
     <row r="14" spans="1:164" s="11" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="78" t="b">
+      <c r="A14" s="72" t="b">
         <v>0</v>
       </c>
-      <c r="B14" s="73"/>
+      <c r="B14" s="74"/>
       <c r="C14" s="23" t="s">
         <v>244</v>
       </c>
@@ -7376,9 +7326,7 @@
       <c r="E14" s="16" t="s">
         <v>208</v>
       </c>
-      <c r="F14" s="16" t="s">
-        <v>301</v>
-      </c>
+      <c r="F14" s="16"/>
       <c r="G14" s="16" t="s">
         <v>162</v>
       </c>
@@ -7709,10 +7657,10 @@
       <c r="FH14" s="27"/>
     </row>
     <row r="15" spans="1:164" s="11" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="78" t="b">
+      <c r="A15" s="72" t="b">
         <v>0</v>
       </c>
-      <c r="B15" s="73"/>
+      <c r="B15" s="74"/>
       <c r="C15" s="23" t="s">
         <v>183</v>
       </c>
@@ -7722,9 +7670,7 @@
       <c r="E15" s="16" t="s">
         <v>209</v>
       </c>
-      <c r="F15" s="16" t="s">
-        <v>301</v>
-      </c>
+      <c r="F15" s="16"/>
       <c r="G15" s="16" t="s">
         <v>162</v>
       </c>
@@ -8027,10 +7973,10 @@
       <c r="FH15" s="27"/>
     </row>
     <row r="16" spans="1:164" s="11" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="78" t="b">
+      <c r="A16" s="72" t="b">
         <v>0</v>
       </c>
-      <c r="B16" s="73"/>
+      <c r="B16" s="74"/>
       <c r="C16" s="23" t="s">
         <v>268</v>
       </c>
@@ -8040,9 +7986,7 @@
       <c r="E16" s="16" t="s">
         <v>210</v>
       </c>
-      <c r="F16" s="16" t="s">
-        <v>301</v>
-      </c>
+      <c r="F16" s="16"/>
       <c r="G16" s="16" t="s">
         <v>162</v>
       </c>
@@ -8345,10 +8289,10 @@
       <c r="FH16" s="27"/>
     </row>
     <row r="17" spans="1:164" s="11" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="78" t="b">
+      <c r="A17" s="72" t="b">
         <v>0</v>
       </c>
-      <c r="B17" s="73"/>
+      <c r="B17" s="74"/>
       <c r="C17" s="23" t="s">
         <v>269</v>
       </c>
@@ -8358,9 +8302,7 @@
       <c r="E17" s="16" t="s">
         <v>211</v>
       </c>
-      <c r="F17" s="16" t="s">
-        <v>301</v>
-      </c>
+      <c r="F17" s="16"/>
       <c r="G17" s="16" t="s">
         <v>162</v>
       </c>
@@ -8667,10 +8609,10 @@
       <c r="FH17" s="27"/>
     </row>
     <row r="18" spans="1:164" s="11" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="78" t="b">
+      <c r="A18" s="72" t="b">
         <v>0</v>
       </c>
-      <c r="B18" s="73"/>
+      <c r="B18" s="74"/>
       <c r="C18" s="23" t="s">
         <v>231</v>
       </c>
@@ -8680,9 +8622,7 @@
       <c r="E18" s="16" t="s">
         <v>212</v>
       </c>
-      <c r="F18" s="16" t="s">
-        <v>301</v>
-      </c>
+      <c r="F18" s="16"/>
       <c r="G18" s="16" t="s">
         <v>162</v>
       </c>
@@ -8993,12 +8933,12 @@
       <c r="FH18" s="27"/>
     </row>
     <row r="19" spans="1:164" s="11" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="78" t="b">
+      <c r="A19" s="72" t="b">
         <v>0</v>
       </c>
-      <c r="B19" s="73"/>
+      <c r="B19" s="74"/>
       <c r="C19" s="23" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D19" s="24" t="s">
         <v>140</v>
@@ -9006,9 +8946,7 @@
       <c r="E19" s="16" t="s">
         <v>213</v>
       </c>
-      <c r="F19" s="16" t="s">
-        <v>301</v>
-      </c>
+      <c r="F19" s="16"/>
       <c r="G19" s="16" t="s">
         <v>162</v>
       </c>
@@ -9327,10 +9265,10 @@
       <c r="FH19" s="27"/>
     </row>
     <row r="20" spans="1:164" s="11" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="78" t="b">
+      <c r="A20" s="72" t="b">
         <v>0</v>
       </c>
-      <c r="B20" s="73"/>
+      <c r="B20" s="74"/>
       <c r="C20" s="23" t="s">
         <v>299</v>
       </c>
@@ -9340,9 +9278,7 @@
       <c r="E20" s="16" t="s">
         <v>233</v>
       </c>
-      <c r="F20" s="16" t="s">
-        <v>301</v>
-      </c>
+      <c r="F20" s="16"/>
       <c r="G20" s="16" t="s">
         <v>162</v>
       </c>
@@ -9679,10 +9615,10 @@
       </c>
     </row>
     <row r="21" spans="1:164" s="11" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="78" t="b">
+      <c r="A21" s="72" t="b">
         <v>0</v>
       </c>
-      <c r="B21" s="74"/>
+      <c r="B21" s="75"/>
       <c r="C21" s="37" t="s">
         <v>300</v>
       </c>
@@ -9692,9 +9628,7 @@
       <c r="E21" s="16" t="s">
         <v>234</v>
       </c>
-      <c r="F21" s="17" t="s">
-        <v>301</v>
-      </c>
+      <c r="F21" s="17"/>
       <c r="G21" s="17" t="s">
         <v>162</v>
       </c>
@@ -10033,11 +9967,11 @@
       </c>
     </row>
     <row r="22" spans="1:164" s="11" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="78" t="b">
+      <c r="A22" s="72" t="b">
         <v>1</v>
       </c>
-      <c r="B22" s="75" t="s">
-        <v>312</v>
+      <c r="B22" s="76" t="s">
+        <v>311</v>
       </c>
       <c r="C22" s="45" t="s">
         <v>270</v>
@@ -10048,9 +9982,7 @@
       <c r="E22" s="46" t="s">
         <v>235</v>
       </c>
-      <c r="F22" s="18" t="s">
-        <v>301</v>
-      </c>
+      <c r="F22" s="18"/>
       <c r="G22" s="18" t="s">
         <v>162</v>
       </c>
@@ -10155,8 +10087,12 @@
       <c r="BF22" s="18"/>
       <c r="BG22" s="18"/>
       <c r="BH22" s="47"/>
-      <c r="BI22" s="47"/>
-      <c r="BJ22" s="47"/>
+      <c r="BI22" s="47" t="s">
+        <v>315</v>
+      </c>
+      <c r="BJ22" s="47" t="s">
+        <v>316</v>
+      </c>
       <c r="BK22" s="18"/>
       <c r="BL22" s="18"/>
       <c r="BM22" s="18"/>
@@ -10389,12 +10325,12 @@
       </c>
     </row>
     <row r="23" spans="1:164" s="11" customFormat="1" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="78" t="b">
+      <c r="A23" s="72" t="b">
         <v>1</v>
       </c>
-      <c r="B23" s="76"/>
+      <c r="B23" s="77"/>
       <c r="C23" s="53" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D23" s="54" t="s">
         <v>140</v>
@@ -10402,14 +10338,12 @@
       <c r="E23" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="F23" s="19" t="s">
-        <v>301</v>
-      </c>
+      <c r="F23" s="19"/>
       <c r="G23" s="19" t="s">
         <v>162</v>
       </c>
       <c r="H23" s="21" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="I23" s="21" t="s">
         <v>142</v>
@@ -10464,11 +10398,11 @@
         <v>279</v>
       </c>
       <c r="AA23" s="19" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AB23" s="19"/>
       <c r="AC23" s="19" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="AD23" s="19" t="s">
         <v>246</v>
@@ -10701,10 +10635,10 @@
       <c r="FH23" s="56"/>
     </row>
     <row r="24" spans="1:164" s="11" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="78" t="b">
+      <c r="A24" s="72" t="b">
         <v>1</v>
       </c>
-      <c r="B24" s="76"/>
+      <c r="B24" s="77"/>
       <c r="C24" s="53" t="s">
         <v>253</v>
       </c>
@@ -10714,9 +10648,7 @@
       <c r="E24" s="19" t="s">
         <v>237</v>
       </c>
-      <c r="F24" s="19" t="s">
-        <v>301</v>
-      </c>
+      <c r="F24" s="19"/>
       <c r="G24" s="19" t="s">
         <v>162</v>
       </c>
@@ -11007,10 +10939,10 @@
       <c r="FH24" s="56"/>
     </row>
     <row r="25" spans="1:164" s="11" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="78" t="b">
+      <c r="A25" s="72" t="b">
         <v>1</v>
       </c>
-      <c r="B25" s="76"/>
+      <c r="B25" s="77"/>
       <c r="C25" s="53" t="s">
         <v>257</v>
       </c>
@@ -11020,9 +10952,7 @@
       <c r="E25" s="19" t="s">
         <v>238</v>
       </c>
-      <c r="F25" s="19" t="s">
-        <v>301</v>
-      </c>
+      <c r="F25" s="19"/>
       <c r="G25" s="19" t="s">
         <v>162</v>
       </c>
@@ -11347,10 +11277,10 @@
       <c r="FH25" s="56"/>
     </row>
     <row r="26" spans="1:164" s="11" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="78" t="b">
+      <c r="A26" s="72" t="b">
         <v>1</v>
       </c>
-      <c r="B26" s="76"/>
+      <c r="B26" s="77"/>
       <c r="C26" s="53" t="s">
         <v>258</v>
       </c>
@@ -11358,11 +11288,9 @@
         <v>140</v>
       </c>
       <c r="E26" s="19" t="s">
-        <v>309</v>
-      </c>
-      <c r="F26" s="19" t="s">
-        <v>301</v>
-      </c>
+        <v>308</v>
+      </c>
+      <c r="F26" s="19"/>
       <c r="G26" s="19" t="s">
         <v>162</v>
       </c>
@@ -11413,7 +11341,7 @@
         <v>164</v>
       </c>
       <c r="X26" s="19" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="Y26" s="19" t="s">
         <v>146</v>
@@ -11665,10 +11593,10 @@
       <c r="FH26" s="56"/>
     </row>
     <row r="27" spans="1:164" s="11" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="78" t="b">
+      <c r="A27" s="72" t="b">
         <v>1</v>
       </c>
-      <c r="B27" s="77"/>
+      <c r="B27" s="78"/>
       <c r="C27" s="59" t="s">
         <v>263</v>
       </c>
@@ -11676,11 +11604,9 @@
         <v>140</v>
       </c>
       <c r="E27" s="20" t="s">
-        <v>313</v>
-      </c>
-      <c r="F27" s="20" t="s">
-        <v>301</v>
-      </c>
+        <v>312</v>
+      </c>
+      <c r="F27" s="20"/>
       <c r="G27" s="20" t="s">
         <v>162</v>
       </c>
@@ -11731,7 +11657,7 @@
         <v>164</v>
       </c>
       <c r="X27" s="20" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="Y27" s="20" t="s">
         <v>146</v>

</xml_diff>